<commit_message>
Google Maps on single page
 - Plot house location on google maps.

Signed-off-by: Thaynara Silva <silvathaynara21@gmail.com>
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18625"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
   <workbookPr date1904="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -81,7 +81,7 @@
     <t>Total</t>
   </si>
   <si>
-    <t>Most popular properties on gallery page.</t>
+    <t>Most popular properties on gallery page. Similar Houses based on location on single page.</t>
   </si>
 </sst>
 </file>
@@ -1602,8 +1602,8 @@
   </sheetPr>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B28" sqref="B28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="21.7" customHeight="1"/>
@@ -1652,7 +1652,7 @@
     </row>
     <row r="5" spans="1:3" ht="36.75" customHeight="1">
       <c r="A5" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B5" s="10" t="s">
         <v>6</v>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="C24" s="30">
         <f>SUMIF(A4:A23,TRUE,C4:C23)</f>
-        <v>0.21</v>
+        <v>0.29000000000000004</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working on edit property functionality
Signed-off-by: Thaynara Silva <silvathaynara21@gmail.com>
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1602,8 +1602,8 @@
   </sheetPr>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="21.7" customHeight="1"/>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="19" spans="1:3" ht="22.8" customHeight="1">
       <c r="A19" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B19" s="23">
         <v>41663.75</v>
@@ -1842,7 +1842,7 @@
       </c>
       <c r="C24" s="30">
         <f>SUMIF(A4:A23,TRUE,C4:C23)</f>
-        <v>0.47000000000000008</v>
+        <v>0.50000000000000011</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Working Edit Vendor details
Signed-off-by: Thaynara Silva <silvathaynara21@gmail.com>
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1602,8 +1602,8 @@
   </sheetPr>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.265625" defaultRowHeight="21.7" customHeight="1"/>
@@ -1723,7 +1723,7 @@
     </row>
     <row r="12" spans="1:3" ht="22.8" customHeight="1">
       <c r="A12" s="12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B12" s="13" t="s">
         <v>13</v>
@@ -1829,9 +1829,7 @@
       <c r="C22" s="18"/>
     </row>
     <row r="23" spans="1:3" ht="22.9" customHeight="1">
-      <c r="A23" s="25" t="b">
-        <v>0</v>
-      </c>
+      <c r="A23" s="25"/>
       <c r="B23" s="26"/>
       <c r="C23" s="27"/>
     </row>
@@ -1842,7 +1840,7 @@
       </c>
       <c r="C24" s="30">
         <f>SUMIF(A4:A23,TRUE,C4:C23)</f>
-        <v>0.50000000000000011</v>
+        <v>0.57000000000000006</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add display report functionality
Signed-off-by: Thaynara Silva <silvathaynara21@gmail.com>
</commit_message>
<xml_diff>
--- a/Checklist.xlsx
+++ b/Checklist.xlsx
@@ -1602,7 +1602,7 @@
   </sheetPr>
   <dimension ref="A1:IV24"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
@@ -1692,7 +1692,7 @@
     </row>
     <row r="9" spans="1:3" ht="22.8" customHeight="1">
       <c r="A9" s="9" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>10</v>

</xml_diff>